<commit_message>
Change of PERMANOVA output to excel. Combining boxplot for bioregions into figure and doing PERMANOVA for bioregions. New boxplot made in new script for different density and biomass calculations. Mean calculations for new boxplot. Updated mean calculations for main data.
</commit_message>
<xml_diff>
--- a/Tables/UNI_PERM_Richness_Boxplot.xlsx
+++ b/Tables/UNI_PERM_Richness_Boxplot.xlsx
@@ -386,19 +386,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.57658610808061</v>
+        <v>1.99007531613154</v>
       </c>
       <c r="C2" t="n">
-        <v>2.57658610808061</v>
+        <v>1.99007531613154</v>
       </c>
       <c r="D2" t="n">
-        <v>2.34335772134836</v>
+        <v>2.79809603102731</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0158030218737724</v>
+        <v>0.0122057646948616</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1291</v>
+        <v>0.1038</v>
       </c>
     </row>
     <row r="3">
@@ -406,70 +406,150 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.99007531613154</v>
+        <v>2.57658610808061</v>
       </c>
       <c r="C3" t="n">
-        <v>1.99007531613154</v>
+        <v>2.57658610808061</v>
       </c>
       <c r="D3" t="n">
-        <v>1.8099369330201</v>
+        <v>3.6227449806447</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0122057646948616</v>
+        <v>0.0158030218737724</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1757</v>
+        <v>0.0578</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.145274435574547</v>
+        <v>24.8358273201153</v>
       </c>
       <c r="C4" t="n">
-        <v>0.145274435574547</v>
+        <v>8.27860910670511</v>
       </c>
       <c r="D4" t="n">
-        <v>0.132124429783461</v>
+        <v>11.6399329694349</v>
       </c>
       <c r="E4" t="n">
-        <v>0.000891014306055814</v>
+        <v>0.152326025962078</v>
       </c>
       <c r="F4" t="n">
-        <v>0.714</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>158.331950851328</v>
+        <v>0.145274435574549</v>
       </c>
       <c r="C5" t="n">
-        <v>1.09952743646756</v>
-      </c>
-      <c r="D5"/>
+        <v>0.145274435574549</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.204259516358933</v>
+      </c>
       <c r="E5" t="n">
-        <v>0.97110019912531</v>
-      </c>
-      <c r="F5"/>
+        <v>0.00089101430605583</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.6475</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.95191573660156</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.317305245533853</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.446139169183954</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.00583840189168323</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7173</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="n">
+        <v>38.4866673488115</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12.8288891162705</v>
+      </c>
+      <c r="D7" t="n">
+        <v>18.0377412994118</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.236050968393578</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.175865615319353</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0586218717731176</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0824238285908722</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.00107863973845861</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9698</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>132</v>
+      </c>
+      <c r="B9" t="n">
+        <v>93.8816748304804</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.711224809321821</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9" t="n">
+        <v>0.575806163139512</v>
+      </c>
+      <c r="F9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
         <v>147</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B10" t="n">
         <v>163.043886711115</v>
       </c>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6" t="n">
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10" t="n">
         <v>1</v>
       </c>
-      <c r="F6"/>
+      <c r="F10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>